<commit_message>
H2n hp hq hr hs ML + SHAP
</commit_message>
<xml_diff>
--- a/hydrogen_comps/Hn_SHAP.xlsx
+++ b/hydrogen_comps/Hn_SHAP.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,410 +447,410 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$(\eta_{q})_{0}$</t>
+          <t>$\eta_{q}$</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.0003433195116428068</v>
+        <v>0.0003120286528607469</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$(\eta_{s})_{0}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{3}$</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.0001485491033298888</v>
+        <v>0.000178705119944324</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{3}$</t>
+          <t>$F_{q}^{\text{SCF}}$</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.0001457584792612691</v>
+        <v>0.0001663771210150696</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$(F_{q}^{\text{SCF}})_{0}$</t>
+          <t>typ_3</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.0001419916070895905</v>
+        <v>0.0001482518102613714</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>typ_0</t>
+          <t>$F_{q}$</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>9.638163317073683e-05</v>
+        <v>7.676449003071209e-05</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>typ_3</t>
+          <t>typ_0</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7.772547922747647e-05</v>
+        <v>7.08917394265382e-05</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>$(F_{q})_{0}$</t>
+          <t>h$_{p}^{3}$</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>6.957920973756573e-05</v>
+        <v>5.368777027915917e-05</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{2}$</t>
+          <t>$F_{s}^{\text{SCF}}$</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>6.628957786118115e-05</v>
+        <v>5.006939112034948e-05</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>typ_1</t>
+          <t>$\eta_{s}$</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>5.887473958055961e-05</v>
+        <v>4.543122173875491e-05</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>$(F_{s})_{0}$</t>
+          <t>typ_1</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2.751802102205239e-05</v>
+        <v>4.357301129632939e-05</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>$(F_{s}^{\text{SCF}})_{0}$</t>
+          <t>h$_{q}$</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2.742621206046463e-05</v>
+        <v>3.234161797869729e-05</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{2}$</t>
+          <t>$\langle ss \vert ss \rangle$</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2.438081560021022e-05</v>
+        <v>3.228634951499118e-05</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>$(\langle qq \vert qq \rangle)_{0}$</t>
+          <t>$F_{s}$</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.398968193223657e-05</v>
+        <v>3.136996949091971e-05</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{2}$</t>
+          <t>typ_2</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2.264406680087902e-05</v>
+        <v>2.862567436174045e-05</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{1}$</t>
+          <t>$\langle qq \vert qq \rangle$</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2.079672563439161e-05</v>
+        <v>2.417239238676062e-05</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>$(\langle ss \vert ss \rangle)_{0}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1.660330379097619e-05</v>
+        <v>2.38385537360706e-05</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{2}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1.659005197244042e-05</v>
+        <v>2.173151209701393e-05</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{2}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1.615505240222782e-05</v>
+        <v>2.031508307183489e-05</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{2}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1.607254622357437e-05</v>
+        <v>1.963358181341187e-05</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{3}$</t>
+          <t>h$_{s}$</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1.551167860324349e-05</v>
+        <v>1.787075992683644e-05</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>typ_2</t>
+          <t>$(\langle pq \vert pq \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1.533297799485518e-05</v>
+        <v>1.773657872936612e-05</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{3}$</t>
+          <t>h$_{p}^{0}$</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1.470377440897387e-05</v>
+        <v>1.442082093653015e-05</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>81</v>
+        <v>1</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{2}$</t>
+          <t>h$_{p}^{1}$</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1.3496382126809e-05</v>
+        <v>1.374466796451365e-05</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>$(F_{p})_{2}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1.027946016403415e-05</v>
+        <v>1.331818415167995e-05</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>$(F_{r})_{2}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1.014818664171306e-05</v>
+        <v>1.272090681041621e-05</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{3}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>9.132569813013124e-06</v>
+        <v>1.212849426293073e-05</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{3}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{1}$</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>8.890793776351148e-06</v>
+        <v>1.076028442801416e-05</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>$(F_{r})_{1}$</t>
+          <t>$(F_{p})_{2}$</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>8.287914235619525e-06</v>
+        <v>1.024076542696946e-05</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{3}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>8.093091703662818e-06</v>
+        <v>9.518002630355294e-06</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{0}$</t>
+          <t>h$_{r}^{3}$</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>7.839647846642931e-06</v>
+        <v>9.356148685667165e-06</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{2}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>7.716010974407162e-06</v>
+        <v>8.997297885239433e-06</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -858,155 +858,155 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>7.417864850101713e-06</v>
+        <v>8.25846854331526e-06</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{0}$</t>
+          <t>h$_{r}^{2}$</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>7.291383406947029e-06</v>
+        <v>8.102123369450462e-06</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{0}$</t>
+          <t>h$_{r}^{1}$</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>6.636728078127451e-06</v>
+        <v>7.981534102196352e-06</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>$(F_{r})_{0}$</t>
+          <t>$(F_{r})_{2}$</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>6.614745482600117e-06</v>
+        <v>7.917595324126087e-06</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>h$_{pr}^{0}$</t>
+          <t>$(\eta_{r})_{3}$</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>6.566902148138141e-06</v>
+        <v>7.847235336701315e-06</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>$(F_{p})_{0}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{2}$</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>6.35464605234787e-06</v>
+        <v>7.560644899364195e-06</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{0}$</t>
+          <t>$(\eta_{r})_{1}$</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>6.073795332579315e-06</v>
+        <v>7.330643990857051e-06</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>h$_{pq}^{1}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{2}$</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>6.02661658151883e-06</v>
+        <v>7.15268754714015e-06</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>$(F_{r})_{3}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>6.007669910583204e-06</v>
+        <v>7.040929584062089e-06</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{3}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>5.75180548935275e-06</v>
+        <v>6.66841315953889e-06</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{1}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{0}$</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>5.415138012494002e-06</v>
+        <v>6.152865975126822e-06</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{2}$</t>
+          <t>h$_{pr}^{2}$</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>5.081989206444637e-06</v>
+        <v>4.445874643769922e-06</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -1014,207 +1014,207 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>5.016954946629461e-06</v>
+        <v>4.362567800006822e-06</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>74</v>
+        <v>2</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{1}$</t>
+          <t>h$_{p}^{2}$</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>4.886871152750697e-06</v>
+        <v>4.310744233912038e-06</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>h$_{pr}^{1}$</t>
+          <t>$(F_{r})_{3}$</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>4.72716677715372e-06</v>
+        <v>4.267214582041578e-06</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>h$_{pq}^{0}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>4.478737390118638e-06</v>
+        <v>4.130051155734099e-06</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{0}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>4.25640737235685e-06</v>
+        <v>3.932411834550611e-06</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>$(F_{p})_{3}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{1}$</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>4.123666313774192e-06</v>
+        <v>3.759495177645263e-06</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>h$_{pr}^{2}$</t>
+          <t>h$_{qs}$</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4.120003760185428e-06</v>
+        <v>3.537733942858679e-06</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>h$_{qs}$</t>
+          <t>$(\eta_{r})_{2}$</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>4.000446347224835e-06</v>
+        <v>3.537179404609569e-06</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{3}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>3.890652143589535e-06</v>
+        <v>3.421562340607928e-06</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{1}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{0}$</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>3.005458136596604e-06</v>
+        <v>3.404712358778438e-06</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{3}$</t>
+          <t>FA$_{qs}$</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>2.51031344646363e-06</v>
+        <v>3.241464679181416e-06</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>h$_{rs}^{3}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2.321655538298049e-06</v>
+        <v>2.838194561741588e-06</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{0}$</t>
+          <t>$(\eta_{r})_{0}$</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2.320189254610753e-06</v>
+        <v>2.704725513205137e-06</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{1}$</t>
+          <t>h$_{pq}^{1}$</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>2.254928848031889e-06</v>
+        <v>2.659346595383147e-06</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{1}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>2.136007795693708e-06</v>
+        <v>2.614005748036462e-06</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>h$_{pq}^{3}$</t>
+          <t>h$_{pr}^{0}$</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2.082038745201618e-06</v>
+        <v>2.479607467253452e-06</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -1222,20 +1222,20 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>2.004956248721741e-06</v>
+        <v>2.449647495229429e-06</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{0}$</t>
+          <t>h$_{r}^{0}$</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1.951502592969994e-06</v>
+        <v>2.371546703376672e-06</v>
       </c>
     </row>
     <row r="63">
@@ -1244,120 +1244,120 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{0}$</t>
+          <t>FI$_{qs}$</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1.766410888716406e-06</v>
+        <v>2.335690635923765e-06</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>FI$_{qs}$</t>
+          <t>h$_{pr}^{1}$</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1.571494764467106e-06</v>
+        <v>2.288690260890244e-06</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{1}$</t>
+          <t>$(F_{r})_{1}$</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1.419726315849026e-06</v>
+        <v>2.263225085330519e-06</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>h$_{rs}^{1}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1.366931808491634e-06</v>
+        <v>2.145851717958019e-06</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{1}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1.320970386461213e-06</v>
+        <v>1.896513055380428e-06</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{0}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1.307348300819799e-06</v>
+        <v>1.670801428923837e-06</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{2}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1.15266421601412e-06</v>
+        <v>1.350615602234156e-06</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{1}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>9.968137785580265e-07</v>
+        <v>1.305967260541634e-06</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{0}$</t>
+          <t>h$_{rs}^{1}$</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>9.741740556058155e-07</v>
+        <v>1.262321325881062e-06</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -1365,318 +1365,448 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>9.293876383131824e-07</v>
+        <v>1.253698157182086e-06</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>FA$_{qs}$</t>
+          <t>$(F_{p})_{3}$</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>8.728571852221859e-07</v>
+        <v>1.134159766282181e-06</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>h$_{pq}^{2}$</t>
+          <t>$(F_{p})_{0}$</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>3.305371689494536e-07</v>
+        <v>1.035296316634328e-06</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{1}$</t>
+          <t>h$_{rs}^{3}$</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1.736736948774395e-07</v>
+        <v>1.007470985340615e-06</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
+          <t>$(F_{r})_{0}$</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>2.678045172891064e-08</v>
+        <v>8.911534250095301e-07</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{3}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>2.371096181185885e-08</v>
+        <v>8.257224378778761e-07</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
+          <t>h$_{pq}^{3}$</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>2.172980171996723e-08</v>
+        <v>7.115247225955786e-07</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
+          <t>h$_{pq}^{0}$</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>1.734540901495105e-08</v>
+        <v>5.401625542421741e-07</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>$(\omega_{s})_{0}$</t>
+          <t>h$_{pq}^{2}$</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>1.492684118652456e-08</v>
+        <v>4.930911223777858e-07</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>$(\omega_{q})_{0}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>1.349816332465259e-08</v>
+        <v>4.897119164922455e-07</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>18</v>
+        <v>103</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>F$_{qs}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>1.335936761132715e-08</v>
+        <v>4.249291055627494e-07</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{2}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1.25196780850224e-08</v>
+        <v>4.187686616701377e-07</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{1}$</t>
+          <t>F$_{qs}$</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>1.229829270217928e-08</v>
+        <v>3.612894512573236e-07</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>h$_{rs}^{2}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>1.209812759016767e-08</v>
+        <v>3.094677282878868e-07</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{3}$</t>
+          <t>h$_{rs}^{2}$</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1.175262536598427e-08</v>
+        <v>1.392854293199905e-07</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>$\mathbf{b}$</t>
+          <t>$(\omega_{r})_{1}$</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>8.510821729927127e-09</v>
+        <v>4.873906685370535e-09</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{0}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>7.319884261027557e-09</v>
+        <v>3.479331468582472e-09</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{3}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>3.381015581048794e-09</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{2}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>3.314632025842405e-09</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{1}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>3.052297388638264e-09</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{0}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>2.565934071740561e-09</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>$(\eta_{p})_{3}$</t>
+          <t>$(\omega_{r})_{0}$</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>2.321984582175945e-09</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>$(\eta_{p})_{2}$</t>
+          <t>$(\omega_{r})_{3}$</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>1.864272165083069e-09</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>$(\eta_{p})_{1}$</t>
+          <t>$\omega_{q}$</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0</v>
+        <v>1.800223016465799e-09</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
+          <t>$(\omega_{r})_{2}$</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>1.77681453178159e-09</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>$\mathbf{b}$</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>1.3374291893842e-09</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>$\omega_{s}$</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>8.674742858625584e-10</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>$(\omega_{p})_{3}$</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>$(\omega_{p})_{2}$</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>$(\omega_{p})_{1}$</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>$(\omega_{p})_{0}$</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>$(\eta_{p})_{3}$</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>$(\eta_{p})_{2}$</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>$(\eta_{p})_{1}$</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
           <t>$(\eta_{p})_{0}$</t>
         </is>
       </c>
-      <c r="C96" t="n">
+      <c r="C106" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Thu Dec 12 04:20:47 PM EST 2024
</commit_message>
<xml_diff>
--- a/hydrogen_comps/Hn_SHAP.xlsx
+++ b/hydrogen_comps/Hn_SHAP.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.0003118887700314612</v>
+        <v>0.0003120172204467836</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.0001781397259310177</v>
+        <v>0.0001778814710337454</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.0001662852796377369</v>
+        <v>0.0001668519649732861</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.0001478796183990289</v>
+        <v>0.0001472818762419537</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>7.730108266176495e-05</v>
+        <v>7.74853219261417e-05</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7.072225907778743e-05</v>
+        <v>7.060314944748904e-05</v>
       </c>
     </row>
     <row r="8">
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5.430832146423747e-05</v>
+        <v>5.401107090161937e-05</v>
       </c>
     </row>
     <row r="9">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4.962405546301033e-05</v>
+        <v>5.009582467455623e-05</v>
       </c>
     </row>
     <row r="10">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>4.573284337043278e-05</v>
+        <v>4.558262841241548e-05</v>
       </c>
     </row>
     <row r="11">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>4.313335713218814e-05</v>
+        <v>4.318485549334553e-05</v>
       </c>
     </row>
     <row r="12">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>3.226105966745889e-05</v>
+        <v>3.236620385005609e-05</v>
       </c>
     </row>
     <row r="13">
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3.224278051786959e-05</v>
+        <v>3.194477308960642e-05</v>
       </c>
     </row>
     <row r="14">
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>3.126320474550945e-05</v>
+        <v>3.128022965747469e-05</v>
       </c>
     </row>
     <row r="15">
@@ -624,7 +624,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2.877003694361847e-05</v>
+        <v>2.812836244031945e-05</v>
       </c>
     </row>
     <row r="16">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2.445022100638185e-05</v>
+        <v>2.437297645613405e-05</v>
       </c>
     </row>
     <row r="17">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2.420290498198948e-05</v>
+        <v>2.428048765225232e-05</v>
       </c>
     </row>
     <row r="18">
@@ -663,7 +663,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2.209112021802153e-05</v>
+        <v>2.154245651384006e-05</v>
       </c>
     </row>
     <row r="19">
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2.021479930922384e-05</v>
+        <v>2.057768493538476e-05</v>
       </c>
     </row>
     <row r="20">
@@ -689,33 +689,33 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1.954536743838997e-05</v>
+        <v>1.965532885650237e-05</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>h$_{s}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1.837484777077044e-05</v>
+        <v>1.817392497424592e-05</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{2}$</t>
+          <t>h$_{s}$</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1.834999725532237e-05</v>
+        <v>1.799234872952975e-05</v>
       </c>
     </row>
     <row r="23">
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1.453672628149277e-05</v>
+        <v>1.426192432767322e-05</v>
       </c>
     </row>
     <row r="24">
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1.393360680686053e-05</v>
+        <v>1.38237298676159e-05</v>
       </c>
     </row>
     <row r="25">
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1.328949816485887e-05</v>
+        <v>1.330714091716932e-05</v>
       </c>
     </row>
     <row r="26">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1.276007444042961e-05</v>
+        <v>1.286163063139556e-05</v>
       </c>
     </row>
     <row r="27">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1.250213705403658e-05</v>
+        <v>1.230002396985267e-05</v>
       </c>
     </row>
     <row r="28">
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1.066306573279862e-05</v>
+        <v>1.083907340948885e-05</v>
       </c>
     </row>
     <row r="29">
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1.038907036863729e-05</v>
+        <v>1.03036158299805e-05</v>
       </c>
     </row>
     <row r="30">
@@ -819,7 +819,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.266555959769003e-06</v>
+        <v>9.369754075793779e-06</v>
       </c>
     </row>
     <row r="31">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>9.152189499449413e-06</v>
+        <v>9.278274433767798e-06</v>
       </c>
     </row>
     <row r="32">
@@ -845,72 +845,72 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>8.98532087842862e-06</v>
+        <v>8.884588843363075e-06</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>h$_{r}^{2}$</t>
+          <t>h$_{pr}^{3}$</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>8.065160204001079e-06</v>
+        <v>8.141327970100411e-06</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>h$_{pr}^{3}$</t>
+          <t>h$_{r}^{2}$</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>8.044672753987536e-06</v>
+        <v>8.09640560594986e-06</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>$(F_{r})_{2}$</t>
+          <t>h$_{r}^{1}$</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>7.952388336634785e-06</v>
+        <v>7.94883774775833e-06</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{3}$</t>
+          <t>$(F_{r})_{2}$</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>7.867454097625458e-06</v>
+        <v>7.8281936721298e-06</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>h$_{r}^{1}$</t>
+          <t>$(\eta_{r})_{3}$</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>7.85792232053566e-06</v>
+        <v>7.75031351713677e-06</v>
       </c>
     </row>
     <row r="38">
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>7.467870389578123e-06</v>
+        <v>7.574674842897949e-06</v>
       </c>
     </row>
     <row r="39">
@@ -936,7 +936,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>7.343825658104257e-06</v>
+        <v>7.33865611703463e-06</v>
       </c>
     </row>
     <row r="40">
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>7.148646912679378e-06</v>
+        <v>7.138719100143492e-06</v>
       </c>
     </row>
     <row r="41">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>7.099900376238455e-06</v>
+        <v>7.098883784052624e-06</v>
       </c>
     </row>
     <row r="42">
@@ -975,7 +975,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>6.77386027587214e-06</v>
+        <v>6.707839937621344e-06</v>
       </c>
     </row>
     <row r="43">
@@ -988,33 +988,33 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>6.222674623542287e-06</v>
+        <v>6.247818660499038e-06</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>h$_{pr}^{2}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{3}$</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>4.492668138529599e-06</v>
+        <v>4.435591140395095e-06</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{3}$</t>
+          <t>h$_{pr}^{2}$</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>4.449898943231209e-06</v>
+        <v>4.414613521288797e-06</v>
       </c>
     </row>
     <row r="46">
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>4.340728791400987e-06</v>
+        <v>4.359525421249219e-06</v>
       </c>
     </row>
     <row r="47">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>4.289423327026767e-06</v>
+        <v>4.240598456688464e-06</v>
       </c>
     </row>
     <row r="48">
@@ -1053,7 +1053,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>4.131595526801031e-06</v>
+        <v>4.13665581098624e-06</v>
       </c>
     </row>
     <row r="49">
@@ -1066,7 +1066,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3.887555442751193e-06</v>
+        <v>3.937358021773291e-06</v>
       </c>
     </row>
     <row r="50">
@@ -1079,46 +1079,46 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>3.81037497801942e-06</v>
+        <v>3.706648974165122e-06</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>h$_{qs}$</t>
+          <t>$(\eta_{r})_{2}$</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>3.591123838822769e-06</v>
+        <v>3.563339621298202e-06</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{2}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{0}$</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>3.565291138975011e-06</v>
+        <v>3.545605974376752e-06</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{0}$</t>
+          <t>h$_{qs}$</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>3.551891334615136e-06</v>
+        <v>3.467056567448506e-06</v>
       </c>
     </row>
     <row r="54">
@@ -1131,7 +1131,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>3.463254901519989e-06</v>
+        <v>3.431753266815229e-06</v>
       </c>
     </row>
     <row r="55">
@@ -1144,7 +1144,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>3.337352373214167e-06</v>
+        <v>3.267765764094631e-06</v>
       </c>
     </row>
     <row r="56">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2.881152647829031e-06</v>
+        <v>2.869427316362245e-06</v>
       </c>
     </row>
     <row r="57">
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2.715666979988428e-06</v>
+        <v>2.711234104729075e-06</v>
       </c>
     </row>
     <row r="58">
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>2.702338019377737e-06</v>
+        <v>2.62975976143675e-06</v>
       </c>
     </row>
     <row r="59">
@@ -1196,7 +1196,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>2.580332043251774e-06</v>
+        <v>2.603771348045123e-06</v>
       </c>
     </row>
     <row r="60">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2.54752725070653e-06</v>
+        <v>2.57900315329351e-06</v>
       </c>
     </row>
     <row r="61">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>2.42542193757136e-06</v>
+        <v>2.460173160205581e-06</v>
       </c>
     </row>
     <row r="62">
@@ -1235,7 +1235,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2.347233277984567e-06</v>
+        <v>2.323367225995174e-06</v>
       </c>
     </row>
     <row r="63">
@@ -1248,7 +1248,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>2.309698529587795e-06</v>
+        <v>2.31888980937027e-06</v>
       </c>
     </row>
     <row r="64">
@@ -1261,7 +1261,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2.281874449679191e-06</v>
+        <v>2.298812190535319e-06</v>
       </c>
     </row>
     <row r="65">
@@ -1274,7 +1274,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>2.254730039944992e-06</v>
+        <v>2.294214471601889e-06</v>
       </c>
     </row>
     <row r="66">
@@ -1287,7 +1287,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2.165147949074693e-06</v>
+        <v>2.200308836325464e-06</v>
       </c>
     </row>
     <row r="67">
@@ -1300,7 +1300,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1.950011391421577e-06</v>
+        <v>1.927698869691738e-06</v>
       </c>
     </row>
     <row r="68">
@@ -1313,7 +1313,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1.692988847594261e-06</v>
+        <v>1.694889497391638e-06</v>
       </c>
     </row>
     <row r="69">
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1.378915750247488e-06</v>
+        <v>1.389867104354688e-06</v>
       </c>
     </row>
     <row r="70">
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1.359905999256912e-06</v>
+        <v>1.312886564480988e-06</v>
       </c>
     </row>
     <row r="71">
@@ -1352,7 +1352,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1.29161797144697e-06</v>
+        <v>1.206476478763909e-06</v>
       </c>
     </row>
     <row r="72">
@@ -1365,7 +1365,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>1.168078636953984e-06</v>
+        <v>1.163262892350264e-06</v>
       </c>
     </row>
     <row r="73">
@@ -1378,7 +1378,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>1.106430290609928e-06</v>
+        <v>1.115444055315405e-06</v>
       </c>
     </row>
     <row r="74">
@@ -1391,7 +1391,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1.043145883623677e-06</v>
+        <v>1.029312882318999e-06</v>
       </c>
     </row>
     <row r="75">
@@ -1404,7 +1404,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1.006279276872939e-06</v>
+        <v>1.010561223360137e-06</v>
       </c>
     </row>
     <row r="76">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>9.022175022583541e-07</v>
+        <v>8.977462137763174e-07</v>
       </c>
     </row>
     <row r="77">
@@ -1430,7 +1430,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>8.280717104121611e-07</v>
+        <v>8.345308863706631e-07</v>
       </c>
     </row>
     <row r="78">
@@ -1443,7 +1443,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>6.948170676646976e-07</v>
+        <v>6.829527940751493e-07</v>
       </c>
     </row>
     <row r="79">
@@ -1456,20 +1456,20 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>5.329867695975828e-07</v>
+        <v>5.175440030462878e-07</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>h$_{pq}^{2}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>4.778022980485697e-07</v>
+        <v>5.012189302508587e-07</v>
       </c>
     </row>
     <row r="81">
@@ -1482,33 +1482,33 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>4.732783192100548e-07</v>
+        <v>4.930600012563717e-07</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{1}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>4.633445317042005e-07</v>
+        <v>4.927169212199049e-07</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{1}$</t>
+          <t>h$_{pq}^{2}$</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>4.323634520042012e-07</v>
+        <v>4.732630602851758e-07</v>
       </c>
     </row>
     <row r="84">
@@ -1521,7 +1521,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>3.589822780551269e-07</v>
+        <v>3.603659128482466e-07</v>
       </c>
     </row>
     <row r="85">
@@ -1534,7 +1534,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>2.965535344085337e-07</v>
+        <v>3.188344659274526e-07</v>
       </c>
     </row>
     <row r="86">
@@ -1547,72 +1547,72 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1.432061829802729e-07</v>
+        <v>1.378075761024632e-07</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{1}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>4.241605916505287e-09</v>
+        <v>7.042809793413909e-09</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>4.17926320442017e-09</v>
+        <v>5.859150272481092e-09</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{3}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>3.936474062050386e-09</v>
+        <v>4.363823016639468e-09</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>$\omega_{q}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>3.364059454888307e-09</v>
+        <v>4.282344878950518e-09</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
+          <t>$\mathbf{b}$</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>3.295078401169368e-09</v>
+        <v>3.332878082008583e-09</v>
       </c>
     </row>
     <row r="92">
@@ -1625,85 +1625,85 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>3.165716540497789e-09</v>
+        <v>3.218433671846697e-09</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{3}$</t>
+          <t>$(\omega_{r})_{1}$</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>2.691107607667725e-09</v>
+        <v>3.061761032898048e-09</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>2.140265908335333e-09</v>
+        <v>2.749630212097297e-09</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{1}$</t>
+          <t>$(\omega_{r})_{3}$</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1.905947324686382e-09</v>
+        <v>2.562520862638928e-09</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{2}$</t>
+          <t>$\omega_{s}$</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>1.742038549332982e-09</v>
+        <v>2.053595893905851e-09</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>$\omega_{s}$</t>
+          <t>$(\omega_{r})_{2}$</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>8.187821133219204e-10</v>
+        <v>1.362750414718833e-09</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>$\mathbf{b}$</t>
+          <t>$\omega_{q}$</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7.335696740910069e-10</v>
+        <v>6.135002374218353e-10</v>
       </c>
     </row>
     <row r="99">

</xml_diff>

<commit_message>
Mon Dec 23 09:55:52 PM EST 2024
</commit_message>
<xml_diff>
--- a/hydrogen_comps/Hn_SHAP.xlsx
+++ b/hydrogen_comps/Hn_SHAP.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C106"/>
+  <dimension ref="A1:C103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,7 +447,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -455,12 +455,12 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.0003120172204467836</v>
+        <v>0.0003228168480881741</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -468,12 +468,12 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.0001778814710337454</v>
+        <v>0.0001757919192235365</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.0001668519649732861</v>
+        <v>0.0001684175982379151</v>
       </c>
     </row>
     <row r="5">
@@ -494,12 +494,12 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.0001472818762419537</v>
+        <v>0.0001614176760873454</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>7.74853219261417e-05</v>
+        <v>7.616611178407889e-05</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7.060314944748904e-05</v>
+        <v>6.884141753541184e-05</v>
       </c>
     </row>
     <row r="8">
@@ -533,12 +533,12 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5.401107090161937e-05</v>
+        <v>5.829618810069284e-05</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -546,12 +546,12 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>5.009582467455623e-05</v>
+        <v>5.276825001622845e-05</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>4.558262841241548e-05</v>
+        <v>4.92770499440691e-05</v>
       </c>
     </row>
     <row r="11">
@@ -572,12 +572,12 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>4.318485549334553e-05</v>
+        <v>4.6648632973022e-05</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>3.236620385005609e-05</v>
+        <v>4.022330443025112e-05</v>
       </c>
     </row>
     <row r="13">
@@ -598,103 +598,103 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3.194477308960642e-05</v>
+        <v>2.860528616256885e-05</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>$F_{s}$</t>
+          <t>h$_{s}$</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>3.128022965747469e-05</v>
+        <v>2.699055353781962e-05</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>typ_2</t>
+          <t>$(\langle rr \vert rr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2.812836244031945e-05</v>
+        <v>2.446513382182623e-05</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>$\langle qq \vert qq \rangle$</t>
+          <t>typ_2</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2.437297645613405e-05</v>
+        <v>2.398006577565084e-05</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{2}$</t>
+          <t>$F_{s}$</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2.428048765225232e-05</v>
+        <v>2.39751688967473e-05</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{2}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2.154245651384006e-05</v>
+        <v>2.326566498322432e-05</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{2}$</t>
+          <t>$\langle qq \vert qq \rangle$</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2.057768493538476e-05</v>
+        <v>2.071731492712363e-05</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{3}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1.965532885650237e-05</v>
+        <v>1.971546041169686e-05</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -702,20 +702,20 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1.817392497424592e-05</v>
+        <v>1.712167888788565e-05</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>h$_{s}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1.799234872952975e-05</v>
+        <v>1.70233796800583e-05</v>
       </c>
     </row>
     <row r="23">
@@ -728,38 +728,38 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1.426192432767322e-05</v>
+        <v>1.626628374463195e-05</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>h$_{p}^{1}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1.38237298676159e-05</v>
+        <v>1.456746994870834e-05</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{2}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{1}$</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1.330714091716932e-05</v>
+        <v>1.446257405749155e-05</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -767,142 +767,142 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1.286163063139556e-05</v>
+        <v>1.2611429293089e-05</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>78</v>
+        <v>1</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{0}$</t>
+          <t>h$_{p}^{1}$</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1.230002396985267e-05</v>
+        <v>1.115262998736973e-05</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{1}$</t>
+          <t>$(F_{r})_{2}$</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1.083907340948885e-05</v>
+        <v>1.069003942516143e-05</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>$(F_{p})_{2}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1.03036158299805e-05</v>
+        <v>1.059034009867228e-05</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>h$_{r}^{3}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.369754075793779e-06</v>
+        <v>1.007916715455327e-05</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{1}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{2}$</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>9.278274433767798e-06</v>
+        <v>9.861028937983504e-06</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{3}$</t>
+          <t>h$_{pr}^{3}$</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>8.884588843363075e-06</v>
+        <v>9.337375103200375e-06</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>h$_{pr}^{3}$</t>
+          <t>h$_{r}^{1}$</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>8.141327970100411e-06</v>
+        <v>9.208086540445609e-06</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>h$_{r}^{2}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>8.09640560594986e-06</v>
+        <v>8.532727030397708e-06</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>h$_{r}^{1}$</t>
+          <t>h$_{r}^{2}$</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>7.94883774775833e-06</v>
+        <v>7.959589444409303e-06</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>$(F_{r})_{2}$</t>
+          <t>$(F_{p})_{2}$</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>7.8281936721298e-06</v>
+        <v>7.557167651582284e-06</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -910,488 +910,488 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>7.75031351713677e-06</v>
+        <v>7.192145678397561e-06</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{2}$</t>
+          <t>h$_{r}^{3}$</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>7.574674842897949e-06</v>
+        <v>7.139522789013433e-06</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{1}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>7.33865611703463e-06</v>
+        <v>7.099418161859568e-06</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{2}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>7.138719100143492e-06</v>
+        <v>6.928776660086902e-06</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>101</v>
+        <v>2</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{3}$</t>
+          <t>h$_{p}^{2}$</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>7.098883784052624e-06</v>
+        <v>6.857023355778006e-06</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{3}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{2}$</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>6.707839937621344e-06</v>
+        <v>6.135373991207635e-06</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{0}$</t>
+          <t>h$_{qs}$</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>6.247818660499038e-06</v>
+        <v>5.948442326551092e-06</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{3}$</t>
+          <t>h$_{pr}^{2}$</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>4.435591140395095e-06</v>
+        <v>5.84500775533776e-06</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>h$_{pr}^{2}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>4.414613521288797e-06</v>
+        <v>5.627095204575566e-06</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>h$_{p}^{2}$</t>
+          <t>$(\eta_{r})_{2}$</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>4.359525421249219e-06</v>
+        <v>5.334940184681194e-06</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>$(F_{r})_{3}$</t>
+          <t>$(F_{r})_{0}$</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>4.240598456688464e-06</v>
+        <v>4.682073561920584e-06</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{3}$</t>
+          <t>$(F_{r})_{3}$</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>4.13665581098624e-06</v>
+        <v>4.273479875761272e-06</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{3}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{1}$</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3.937358021773291e-06</v>
+        <v>4.253092636566233e-06</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{1}$</t>
+          <t>$(\eta_{r})_{0}$</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>3.706648974165122e-06</v>
+        <v>3.975515652845992e-06</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{2}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>3.563339621298202e-06</v>
+        <v>3.933079541944607e-06</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{0}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{0}$</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>3.545605974376752e-06</v>
+        <v>3.912934497891247e-06</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>h$_{qs}$</t>
+          <t>h$_{r}^{0}$</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>3.467056567448506e-06</v>
+        <v>3.515735696771053e-06</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{0}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{0}$</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>3.431753266815229e-06</v>
+        <v>3.462981865845538e-06</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>FA$_{qs}$</t>
+          <t>$(F_{p})_{1}$</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>3.267765764094631e-06</v>
+        <v>3.377077806489664e-06</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{0}$</t>
+          <t>$(F_{p})_{3}$</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2.869427316362245e-06</v>
+        <v>3.214137479004373e-06</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{0}$</t>
+          <t>h$_{pr}^{0}$</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2.711234104729075e-06</v>
+        <v>3.060247965499053e-06</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>88</v>
+        <v>30</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{1}$</t>
+          <t>$(F_{p})_{0}$</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>2.62975976143675e-06</v>
+        <v>2.949374490602372e-06</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>h$_{pq}^{1}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>2.603771348045123e-06</v>
+        <v>2.899150800926724e-06</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>h$_{pr}^{0}$</t>
+          <t>h$_{pr}^{1}$</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2.57900315329351e-06</v>
+        <v>2.862516739148026e-06</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>$(F_{p})_{1}$</t>
+          <t>h$_{pq}^{1}$</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>2.460173160205581e-06</v>
+        <v>2.857862325583933e-06</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>FI$_{qs}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2.323367225995174e-06</v>
+        <v>2.781001300597245e-06</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>h$_{r}^{0}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{3}$</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>2.31888980937027e-06</v>
+        <v>2.722756312685238e-06</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>h$_{pr}^{1}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2.298812190535319e-06</v>
+        <v>2.545697617028583e-06</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>$(F_{r})_{1}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>2.294214471601889e-06</v>
+        <v>2.345890791884157e-06</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{0}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2.200308836325464e-06</v>
+        <v>2.271083490447917e-06</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{0}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1.927698869691738e-06</v>
+        <v>2.104788970245593e-06</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{0}$</t>
+          <t>h$_{rs}^{1}$</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1.694889497391638e-06</v>
+        <v>2.09605197999302e-06</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{0}$</t>
+          <t>$(F_{r})_{1}$</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1.389867104354688e-06</v>
+        <v>1.886747489527011e-06</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{1}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1.312886564480988e-06</v>
+        <v>1.600171583190679e-06</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>h$_{rs}^{1}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1.206476478763909e-06</v>
+        <v>1.505254884354509e-06</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>h$_{rs}^{0}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>1.163262892350264e-06</v>
+        <v>1.409126401996057e-06</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>$(F_{p})_{3}$</t>
+          <t>$(\eta_{r})_{1}$</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>1.115444055315405e-06</v>
+        <v>1.408826025321477e-06</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>$(F_{p})_{0}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1.029312882318999e-06</v>
+        <v>1.360577755189295e-06</v>
       </c>
     </row>
     <row r="75">
@@ -1404,46 +1404,46 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1.010561223360137e-06</v>
+        <v>1.294250460882649e-06</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>$(F_{r})_{0}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>8.977462137763174e-07</v>
+        <v>1.16169616892679e-06</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{1}$</t>
+          <t>h$_{rs}^{0}$</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>8.345308863706631e-07</v>
+        <v>9.545999113380304e-07</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>h$_{pq}^{3}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>6.829527940751493e-07</v>
+        <v>7.390335329716462e-07</v>
       </c>
     </row>
     <row r="79">
@@ -1456,263 +1456,263 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>5.175440030462878e-07</v>
+        <v>6.957965758568148e-07</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{1}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>5.012189302508587e-07</v>
+        <v>6.449551890490444e-07</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>103</v>
+        <v>7</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{3}$</t>
+          <t>h$_{pq}^{3}$</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>4.930600012563717e-07</v>
+        <v>5.503630449009169e-07</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{1}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>4.927169212199049e-07</v>
+        <v>3.528300440006637e-07</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>h$_{pq}^{2}$</t>
+          <t>h$_{rs}^{2}$</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>4.732630602851758e-07</v>
+        <v>3.814449586470488e-08</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>F$_{qs}$</t>
+          <t>h$_{pq}^{2}$</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>3.603659128482466e-07</v>
+        <v>1.50559889288841e-08</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{2}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>3.188344659274526e-07</v>
+        <v>4.35451488722858e-09</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>h$_{rs}^{2}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1.378075761024632e-07</v>
+        <v>4.279197869453409e-09</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{3}$</t>
+          <t>$(\omega_{r})_{1}$</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>7.042809793413909e-09</v>
+        <v>1.951870184555301e-09</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
+          <t>$(\omega_{r})_{0}$</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>5.859150272481092e-09</v>
+        <v>1.592892723627807e-09</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
+          <t>$(\omega_{r})_{2}$</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>4.363823016639468e-09</v>
+        <v>1.560024658936236e-09</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{1}$</t>
+          <t>$\omega_{q}$</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>4.282344878950518e-09</v>
+        <v>1.483177499716522e-09</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>$\mathbf{b}$</t>
+          <t>$(\omega_{r})_{3}$</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>3.332878082008583e-09</v>
+        <v>1.471831218133535e-09</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{0}$</t>
+          <t>$\omega_{s}$</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>3.218433671846697e-09</v>
+        <v>1.283397306195144e-09</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{1}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>3.061761032898048e-09</v>
+        <v>1.18939283811566e-09</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>2.749630212097297e-09</v>
+        <v>1.064679887955827e-09</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{3}$</t>
+          <t>$\mathbf{b}$</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>2.562520862638928e-09</v>
+        <v>1.108429643910596e-10</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>$\omega_{s}$</t>
+          <t>$(\omega_{p})_{3}$</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>2.053595893905851e-09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{2}$</t>
+          <t>$(\omega_{p})_{2}$</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>1.362750414718833e-09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>$\omega_{q}$</t>
+          <t>$(\omega_{p})_{1}$</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>6.135002374218353e-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{3}$</t>
+          <t>$(\omega_{p})_{0}$</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -1721,11 +1721,11 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{2}$</t>
+          <t>$(\eta_{p})_{3}$</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -1734,11 +1734,11 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{1}$</t>
+          <t>$(\eta_{p})_{2}$</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -1747,11 +1747,11 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{0}$</t>
+          <t>$(\eta_{p})_{1}$</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -1760,53 +1760,14 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>$(\eta_{p})_{3}$</t>
+          <t>$(\eta_{p})_{0}$</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>$(\eta_{p})_{2}$</t>
-        </is>
-      </c>
-      <c r="C104" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>$(\eta_{p})_{1}$</t>
-        </is>
-      </c>
-      <c r="C105" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>$(\eta_{p})_{0}$</t>
-        </is>
-      </c>
-      <c r="C106" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tue Dec 24 10:40:06 AM EST 2024 figures
</commit_message>
<xml_diff>
--- a/hydrogen_comps/Hn_SHAP.xlsx
+++ b/hydrogen_comps/Hn_SHAP.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.0003228168480881741</v>
+        <v>0.000323319659290534</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.0001757919192235365</v>
+        <v>0.0001757085724566559</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.0001684175982379151</v>
+        <v>0.000167343829378347</v>
       </c>
     </row>
     <row r="5">
@@ -490,11 +490,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>typ_3</t>
+          <t>type_3</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.0001614176760873454</v>
+        <v>0.0001615497839389279</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>7.616611178407889e-05</v>
+        <v>7.593560334400594e-05</v>
       </c>
     </row>
     <row r="7">
@@ -516,11 +516,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>typ_0</t>
+          <t>type_0</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>6.884141753541184e-05</v>
+        <v>7.007430859284367e-05</v>
       </c>
     </row>
     <row r="8">
@@ -529,11 +529,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>h$_{p}^{3}$</t>
+          <t>(h$_{p}$)$_{3}$</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5.829618810069284e-05</v>
+        <v>5.815195854567683e-05</v>
       </c>
     </row>
     <row r="9">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>5.276825001622845e-05</v>
+        <v>5.326467721225847e-05</v>
       </c>
     </row>
     <row r="10">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>4.92770499440691e-05</v>
+        <v>4.929968014736198e-05</v>
       </c>
     </row>
     <row r="11">
@@ -568,11 +568,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>typ_1</t>
+          <t>type_1</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>4.6648632973022e-05</v>
+        <v>4.75487959035365e-05</v>
       </c>
     </row>
     <row r="12">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>4.022330443025112e-05</v>
+        <v>3.921608327345163e-05</v>
       </c>
     </row>
     <row r="13">
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2.860528616256885e-05</v>
+        <v>2.824189854324345e-05</v>
       </c>
     </row>
     <row r="14">
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.699055353781962e-05</v>
+        <v>2.715463632106607e-05</v>
       </c>
     </row>
     <row r="15">
@@ -624,7 +624,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2.446513382182623e-05</v>
+        <v>2.455300804959925e-05</v>
       </c>
     </row>
     <row r="16">
@@ -633,11 +633,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>typ_2</t>
+          <t>type_2</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2.398006577565084e-05</v>
+        <v>2.403831982194308e-05</v>
       </c>
     </row>
     <row r="17">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2.39751688967473e-05</v>
+        <v>2.369948219689375e-05</v>
       </c>
     </row>
     <row r="18">
@@ -663,7 +663,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2.326566498322432e-05</v>
+        <v>2.331067635768819e-05</v>
       </c>
     </row>
     <row r="19">
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2.071731492712363e-05</v>
+        <v>2.069220219422768e-05</v>
       </c>
     </row>
     <row r="20">
@@ -689,7 +689,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1.971546041169686e-05</v>
+        <v>1.978033023138282e-05</v>
       </c>
     </row>
     <row r="21">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1.712167888788565e-05</v>
+        <v>1.696587663503903e-05</v>
       </c>
     </row>
     <row r="22">
@@ -715,7 +715,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1.70233796800583e-05</v>
+        <v>1.69295312454462e-05</v>
       </c>
     </row>
     <row r="23">
@@ -724,37 +724,37 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>h$_{p}^{0}$</t>
+          <t>(h$_{p}$)$_{0}$</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1.626628374463195e-05</v>
+        <v>1.647028120560167e-05</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{2}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{1}$</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1.456746994870834e-05</v>
+        <v>1.4399014374284e-05</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{1}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1.446257405749155e-05</v>
+        <v>1.43312779978816e-05</v>
       </c>
     </row>
     <row r="26">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1.2611429293089e-05</v>
+        <v>1.267050212049094e-05</v>
       </c>
     </row>
     <row r="27">
@@ -776,37 +776,37 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>h$_{p}^{1}$</t>
+          <t>(h$_{p}$)$_{1}$</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1.115262998736973e-05</v>
+        <v>1.111874518996097e-05</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>$(F_{r})_{2}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1.069003942516143e-05</v>
+        <v>1.075352999252778e-05</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{2}$</t>
+          <t>$(F_{r})_{2}$</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1.059034009867228e-05</v>
+        <v>1.06922904798782e-05</v>
       </c>
     </row>
     <row r="30">
@@ -819,7 +819,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1.007916715455327e-05</v>
+        <v>9.97856588650984e-06</v>
       </c>
     </row>
     <row r="31">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>9.861028937983504e-06</v>
+        <v>9.880168318315773e-06</v>
       </c>
     </row>
     <row r="32">
@@ -841,11 +841,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>h$_{pr}^{3}$</t>
+          <t>(h$_{pr}$)$_{3}$</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>9.337375103200375e-06</v>
+        <v>9.412418613818235e-06</v>
       </c>
     </row>
     <row r="33">
@@ -854,11 +854,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>h$_{r}^{1}$</t>
+          <t>(h$_{r}$)$_{1}$</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>9.208086540445609e-06</v>
+        <v>9.213635861829751e-06</v>
       </c>
     </row>
     <row r="34">
@@ -871,7 +871,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>8.532727030397708e-06</v>
+        <v>8.669854634485175e-06</v>
       </c>
     </row>
     <row r="35">
@@ -880,11 +880,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>h$_{r}^{2}$</t>
+          <t>(h$_{r}$)$_{2}$</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>7.959589444409303e-06</v>
+        <v>7.999564397386185e-06</v>
       </c>
     </row>
     <row r="36">
@@ -897,33 +897,33 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>7.557167651582284e-06</v>
+        <v>7.554486870731305e-06</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{3}$</t>
+          <t>(h$_{r}$)$_{3}$</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>7.192145678397561e-06</v>
+        <v>7.16988903912837e-06</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>h$_{r}^{3}$</t>
+          <t>$(\eta_{r})_{3}$</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>7.139522789013433e-06</v>
+        <v>7.167021313490361e-06</v>
       </c>
     </row>
     <row r="39">
@@ -936,7 +936,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>7.099418161859568e-06</v>
+        <v>7.018979581569162e-06</v>
       </c>
     </row>
     <row r="40">
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>6.928776660086902e-06</v>
+        <v>6.997121490467267e-06</v>
       </c>
     </row>
     <row r="41">
@@ -958,37 +958,37 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>h$_{p}^{2}$</t>
+          <t>(h$_{p}$)$_{2}$</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>6.857023355778006e-06</v>
+        <v>6.874651434815424e-06</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{2}$</t>
+          <t>h$_{qs}$</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>6.135373991207635e-06</v>
+        <v>6.058142791082416e-06</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>h$_{qs}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{2}$</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>5.948442326551092e-06</v>
+        <v>6.038100453020164e-06</v>
       </c>
     </row>
     <row r="44">
@@ -997,11 +997,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>h$_{pr}^{2}$</t>
+          <t>(h$_{pr}$)$_{2}$</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>5.84500775533776e-06</v>
+        <v>5.866224091976741e-06</v>
       </c>
     </row>
     <row r="45">
@@ -1014,7 +1014,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>5.627095204575566e-06</v>
+        <v>5.584662610670774e-06</v>
       </c>
     </row>
     <row r="46">
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>5.334940184681194e-06</v>
+        <v>5.345206571897236e-06</v>
       </c>
     </row>
     <row r="47">
@@ -1040,72 +1040,72 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>4.682073561920584e-06</v>
+        <v>4.693567335085946e-06</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>$(F_{r})_{3}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{1}$</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>4.273479875761272e-06</v>
+        <v>4.297232637943183e-06</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{1}$</t>
+          <t>$(F_{r})_{3}$</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>4.253092636566233e-06</v>
+        <v>4.267782444560504e-06</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{0}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>3.975515652845992e-06</v>
+        <v>3.967105339601254e-06</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{0}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{0}$</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>3.933079541944607e-06</v>
+        <v>3.935547760671783e-06</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{0}$</t>
+          <t>$(\eta_{r})_{0}$</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>3.912934497891247e-06</v>
+        <v>3.907724065533214e-06</v>
       </c>
     </row>
     <row r="53">
@@ -1114,11 +1114,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>h$_{r}^{0}$</t>
+          <t>(h$_{r}$)$_{0}$</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>3.515735696771053e-06</v>
+        <v>3.553340558405851e-06</v>
       </c>
     </row>
     <row r="54">
@@ -1131,7 +1131,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>3.462981865845538e-06</v>
+        <v>3.514055150533764e-06</v>
       </c>
     </row>
     <row r="55">
@@ -1144,7 +1144,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>3.377077806489664e-06</v>
+        <v>3.43653622366948e-06</v>
       </c>
     </row>
     <row r="56">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>3.214137479004373e-06</v>
+        <v>3.271165589167211e-06</v>
       </c>
     </row>
     <row r="57">
@@ -1166,50 +1166,50 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>h$_{pr}^{0}$</t>
+          <t>(h$_{pr}$)$_{0}$</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>3.060247965499053e-06</v>
+        <v>3.0629944695756e-06</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>$(F_{p})_{0}$</t>
+          <t>(h$_{pr}$)$_{1}$</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>2.949374490602372e-06</v>
+        <v>2.982622927976264e-06</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{0}$</t>
+          <t>$(F_{p})_{0}$</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>2.899150800926724e-06</v>
+        <v>2.912765229541939e-06</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>h$_{pr}^{1}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2.862516739148026e-06</v>
+        <v>2.879258890548974e-06</v>
       </c>
     </row>
     <row r="61">
@@ -1218,37 +1218,37 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>h$_{pq}^{1}$</t>
+          <t>(h$_{pq}$)$_{1}$</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>2.857862325583933e-06</v>
+        <v>2.857746904189719e-06</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>101</v>
+        <v>60</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{3}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{3}$</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2.781001300597245e-06</v>
+        <v>2.74927901996683e-06</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{3}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>2.722756312685238e-06</v>
+        <v>2.69109803998534e-06</v>
       </c>
     </row>
     <row r="64">
@@ -1261,7 +1261,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2.545697617028583e-06</v>
+        <v>2.601342485196746e-06</v>
       </c>
     </row>
     <row r="65">
@@ -1274,7 +1274,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>2.345890791884157e-06</v>
+        <v>2.304631293351454e-06</v>
       </c>
     </row>
     <row r="66">
@@ -1287,7 +1287,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2.271083490447917e-06</v>
+        <v>2.274781968690367e-06</v>
       </c>
     </row>
     <row r="67">
@@ -1300,7 +1300,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>2.104788970245593e-06</v>
+        <v>2.161522061566603e-06</v>
       </c>
     </row>
     <row r="68">
@@ -1309,11 +1309,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>h$_{rs}^{1}$</t>
+          <t>(h$_{rs}$)$_{1}$</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>2.09605197999302e-06</v>
+        <v>2.034060694932896e-06</v>
       </c>
     </row>
     <row r="69">
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1.886747489527011e-06</v>
+        <v>1.867379770044898e-06</v>
       </c>
     </row>
     <row r="70">
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1.600171583190679e-06</v>
+        <v>1.616492031364258e-06</v>
       </c>
     </row>
     <row r="71">
@@ -1352,7 +1352,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1.505254884354509e-06</v>
+        <v>1.541625136547503e-06</v>
       </c>
     </row>
     <row r="72">
@@ -1365,7 +1365,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>1.409126401996057e-06</v>
+        <v>1.420549705372149e-06</v>
       </c>
     </row>
     <row r="73">
@@ -1378,7 +1378,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>1.408826025321477e-06</v>
+        <v>1.419893049000004e-06</v>
       </c>
     </row>
     <row r="74">
@@ -1391,7 +1391,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1.360577755189295e-06</v>
+        <v>1.331841715321663e-06</v>
       </c>
     </row>
     <row r="75">
@@ -1400,11 +1400,11 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>h$_{rs}^{3}$</t>
+          <t>(h$_{rs}$)$_{3}$</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1.294250460882649e-06</v>
+        <v>1.287323041683143e-06</v>
       </c>
     </row>
     <row r="76">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>1.16169616892679e-06</v>
+        <v>1.1524700653601e-06</v>
       </c>
     </row>
     <row r="77">
@@ -1426,11 +1426,11 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>h$_{rs}^{0}$</t>
+          <t>(h$_{rs}$)$_{0}$</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>9.545999113380304e-07</v>
+        <v>9.693119354045891e-07</v>
       </c>
     </row>
     <row r="78">
@@ -1443,7 +1443,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>7.390335329716462e-07</v>
+        <v>7.53046982235866e-07</v>
       </c>
     </row>
     <row r="79">
@@ -1452,11 +1452,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>h$_{pq}^{0}$</t>
+          <t>(h$_{pq}$)$_{0}$</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>6.957965758568148e-07</v>
+        <v>6.791581286895688e-07</v>
       </c>
     </row>
     <row r="80">
@@ -1469,7 +1469,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>6.449551890490444e-07</v>
+        <v>6.365518206814005e-07</v>
       </c>
     </row>
     <row r="81">
@@ -1478,11 +1478,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>h$_{pq}^{3}$</t>
+          <t>(h$_{pq}$)$_{3}$</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>5.503630449009169e-07</v>
+        <v>5.311686981222513e-07</v>
       </c>
     </row>
     <row r="82">
@@ -1495,7 +1495,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>3.528300440006637e-07</v>
+        <v>3.503942292561819e-07</v>
       </c>
     </row>
     <row r="83">
@@ -1504,11 +1504,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>h$_{rs}^{2}$</t>
+          <t>(h$_{rs}$)$_{2}$</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>3.814449586470488e-08</v>
+        <v>3.897830628535145e-08</v>
       </c>
     </row>
     <row r="84">
@@ -1517,11 +1517,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>h$_{pq}^{2}$</t>
+          <t>(h$_{pq}$)$_{2}$</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>1.50559889288841e-08</v>
+        <v>1.084715341690152e-08</v>
       </c>
     </row>
     <row r="85">
@@ -1534,33 +1534,33 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>4.35451488722858e-09</v>
+        <v>3.229006925045185e-09</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
+          <t>$(\omega_{r})_{2}$</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>4.279197869453409e-09</v>
+        <v>2.586757821491536e-09</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{1}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>1.951870184555301e-09</v>
+        <v>1.864466745935933e-09</v>
       </c>
     </row>
     <row r="88">
@@ -1573,33 +1573,33 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>1.592892723627807e-09</v>
+        <v>1.782015059132638e-09</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{2}$</t>
+          <t>$(\omega_{r})_{1}$</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1.560024658936236e-09</v>
+        <v>1.75481771446811e-09</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>$\omega_{q}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>1.483177499716522e-09</v>
+        <v>1.671646071409022e-09</v>
       </c>
     </row>
     <row r="91">
@@ -1612,7 +1612,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>1.471831218133535e-09</v>
+        <v>1.63652090483557e-09</v>
       </c>
     </row>
     <row r="92">
@@ -1625,33 +1625,33 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>1.283397306195144e-09</v>
+        <v>1.450305140952312e-09</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>87</v>
+        <v>33</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
+          <t>$\omega_{q}$</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1.18939283811566e-09</v>
+        <v>1.06117104656905e-09</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1.064679887955827e-09</v>
+        <v>1.049725565464064e-09</v>
       </c>
     </row>
     <row r="95">
@@ -1664,7 +1664,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1.108429643910596e-10</v>
+        <v>2.091820723572891e-10</v>
       </c>
     </row>
     <row r="96">

</xml_diff>

<commit_message>
Mon Feb  3 05:14:05 PM EST 2025
</commit_message>
<xml_diff>
--- a/hydrogen_comps/Hn_SHAP.xlsx
+++ b/hydrogen_comps/Hn_SHAP.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.000323319659290534</v>
+        <v>0.0003227950214445237</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.0001757085724566559</v>
+        <v>0.0001753855856154807</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.000167343829378347</v>
+        <v>0.0001673776427848547</v>
       </c>
     </row>
     <row r="5">
@@ -490,11 +490,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>type_3</t>
+          <t>$type_3$</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.0001615497839389279</v>
+        <v>0.0001610445718908489</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>7.593560334400594e-05</v>
+        <v>7.570715940509855e-05</v>
       </c>
     </row>
     <row r="7">
@@ -516,11 +516,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>type_0</t>
+          <t>$type_0$</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7.007430859284367e-05</v>
+        <v>6.879427968757793e-05</v>
       </c>
     </row>
     <row r="8">
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5.815195854567683e-05</v>
+        <v>5.77540952000027e-05</v>
       </c>
     </row>
     <row r="9">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>5.326467721225847e-05</v>
+        <v>5.263956527928243e-05</v>
       </c>
     </row>
     <row r="10">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>4.929968014736198e-05</v>
+        <v>4.926152601733272e-05</v>
       </c>
     </row>
     <row r="11">
@@ -568,11 +568,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>type_1</t>
+          <t>$type_1$</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>4.75487959035365e-05</v>
+        <v>4.701170733170275e-05</v>
       </c>
     </row>
     <row r="12">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>3.921608327345163e-05</v>
+        <v>3.992743153664366e-05</v>
       </c>
     </row>
     <row r="13">
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2.824189854324345e-05</v>
+        <v>2.815855409680222e-05</v>
       </c>
     </row>
     <row r="14">
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.715463632106607e-05</v>
+        <v>2.696122646959244e-05</v>
       </c>
     </row>
     <row r="15">
@@ -624,33 +624,33 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2.455300804959925e-05</v>
+        <v>2.448931413413242e-05</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>type_2</t>
+          <t>$F_{s}$</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2.403831982194308e-05</v>
+        <v>2.416242784405762e-05</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>$F_{s}$</t>
+          <t>$type_2$</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2.369948219689375e-05</v>
+        <v>2.413045251152342e-05</v>
       </c>
     </row>
     <row r="18">
@@ -663,7 +663,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2.331067635768819e-05</v>
+        <v>2.312587742922136e-05</v>
       </c>
     </row>
     <row r="19">
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2.069220219422768e-05</v>
+        <v>2.047014961696811e-05</v>
       </c>
     </row>
     <row r="20">
@@ -689,7 +689,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1.978033023138282e-05</v>
+        <v>1.962903448433232e-05</v>
       </c>
     </row>
     <row r="21">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1.696587663503903e-05</v>
+        <v>1.725185565443219e-05</v>
       </c>
     </row>
     <row r="22">
@@ -715,7 +715,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1.69295312454462e-05</v>
+        <v>1.704692822557048e-05</v>
       </c>
     </row>
     <row r="23">
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1.647028120560167e-05</v>
+        <v>1.632258485374428e-05</v>
       </c>
     </row>
     <row r="24">
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1.4399014374284e-05</v>
+        <v>1.457445281302858e-05</v>
       </c>
     </row>
     <row r="25">
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1.43312779978816e-05</v>
+        <v>1.439184378747983e-05</v>
       </c>
     </row>
     <row r="26">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1.267050212049094e-05</v>
+        <v>1.25719996788816e-05</v>
       </c>
     </row>
     <row r="27">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1.111874518996097e-05</v>
+        <v>1.114783795951332e-05</v>
       </c>
     </row>
     <row r="28">
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1.075352999252778e-05</v>
+        <v>1.078555204045189e-05</v>
       </c>
     </row>
     <row r="29">
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1.06922904798782e-05</v>
+        <v>1.071578629546989e-05</v>
       </c>
     </row>
     <row r="30">
@@ -819,7 +819,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.97856588650984e-06</v>
+        <v>1.006839772539599e-05</v>
       </c>
     </row>
     <row r="31">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>9.880168318315773e-06</v>
+        <v>9.769173504323023e-06</v>
       </c>
     </row>
     <row r="32">
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>9.412418613818235e-06</v>
+        <v>9.51062918574289e-06</v>
       </c>
     </row>
     <row r="33">
@@ -858,7 +858,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>9.213635861829751e-06</v>
+        <v>9.173416877423239e-06</v>
       </c>
     </row>
     <row r="34">
@@ -871,7 +871,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>8.669854634485175e-06</v>
+        <v>8.678508376483038e-06</v>
       </c>
     </row>
     <row r="35">
@@ -884,7 +884,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>7.999564397386185e-06</v>
+        <v>7.896088743440199e-06</v>
       </c>
     </row>
     <row r="36">
@@ -897,33 +897,33 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>7.554486870731305e-06</v>
+        <v>7.6667606184102e-06</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>(h$_{r}$)$_{3}$</t>
+          <t>$(\eta_{r})_{3}$</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>7.16988903912837e-06</v>
+        <v>7.176969880878323e-06</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{3}$</t>
+          <t>(h$_{r}$)$_{3}$</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>7.167021313490361e-06</v>
+        <v>7.110177598836302e-06</v>
       </c>
     </row>
     <row r="39">
@@ -936,7 +936,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>7.018979581569162e-06</v>
+        <v>6.957688186202625e-06</v>
       </c>
     </row>
     <row r="40">
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>6.997121490467267e-06</v>
+        <v>6.935796939126503e-06</v>
       </c>
     </row>
     <row r="41">
@@ -962,33 +962,33 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>6.874651434815424e-06</v>
+        <v>6.729399788789961e-06</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>h$_{qs}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{2}$</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>6.058142791082416e-06</v>
+        <v>6.061597221617856e-06</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{2}$</t>
+          <t>h$_{qs}$</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>6.038100453020164e-06</v>
+        <v>5.941356018362779e-06</v>
       </c>
     </row>
     <row r="44">
@@ -1001,7 +1001,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>5.866224091976741e-06</v>
+        <v>5.891014227902865e-06</v>
       </c>
     </row>
     <row r="45">
@@ -1014,7 +1014,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>5.584662610670774e-06</v>
+        <v>5.618362713144107e-06</v>
       </c>
     </row>
     <row r="46">
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>5.345206571897236e-06</v>
+        <v>5.338060986601502e-06</v>
       </c>
     </row>
     <row r="47">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>4.693567335085946e-06</v>
+        <v>4.530380903826383e-06</v>
       </c>
     </row>
     <row r="48">
@@ -1053,7 +1053,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>4.297232637943183e-06</v>
+        <v>4.302899165472879e-06</v>
       </c>
     </row>
     <row r="49">
@@ -1066,7 +1066,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>4.267782444560504e-06</v>
+        <v>4.235280167744376e-06</v>
       </c>
     </row>
     <row r="50">
@@ -1079,59 +1079,59 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>3.967105339601254e-06</v>
+        <v>4.069239602619167e-06</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{0}$</t>
+          <t>$(\eta_{r})_{0}$</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>3.935547760671783e-06</v>
+        <v>3.955465183942162e-06</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{0}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{0}$</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>3.907724065533214e-06</v>
+        <v>3.931529687778767e-06</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>(h$_{r}$)$_{0}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{0}$</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>3.553340558405851e-06</v>
+        <v>3.600087842877399e-06</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{0}$</t>
+          <t>(h$_{r}$)$_{0}$</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>3.514055150533764e-06</v>
+        <v>3.531127554336526e-06</v>
       </c>
     </row>
     <row r="55">
@@ -1144,7 +1144,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>3.43653622366948e-06</v>
+        <v>3.48541636278326e-06</v>
       </c>
     </row>
     <row r="56">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>3.271165589167211e-06</v>
+        <v>3.252432154811559e-06</v>
       </c>
     </row>
     <row r="57">
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>3.0629944695756e-06</v>
+        <v>3.202765399077644e-06</v>
       </c>
     </row>
     <row r="58">
@@ -1183,33 +1183,33 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>2.982622927976264e-06</v>
+        <v>2.920699910651781e-06</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>$(F_{p})_{0}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>2.912765229541939e-06</v>
+        <v>2.88424697880187e-06</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{0}$</t>
+          <t>$(F_{p})_{0}$</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2.879258890548974e-06</v>
+        <v>2.882693522547001e-06</v>
       </c>
     </row>
     <row r="61">
@@ -1222,33 +1222,33 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>2.857746904189719e-06</v>
+        <v>2.837365505930205e-06</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{3}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2.74927901996683e-06</v>
+        <v>2.748105365620831e-06</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>101</v>
+        <v>60</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{3}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{3}$</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>2.69109803998534e-06</v>
+        <v>2.69693990239924e-06</v>
       </c>
     </row>
     <row r="64">
@@ -1261,7 +1261,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2.601342485196746e-06</v>
+        <v>2.51334631288551e-06</v>
       </c>
     </row>
     <row r="65">
@@ -1274,7 +1274,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>2.304631293351454e-06</v>
+        <v>2.439737469507662e-06</v>
       </c>
     </row>
     <row r="66">
@@ -1287,33 +1287,33 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2.274781968690367e-06</v>
+        <v>2.168225676520742e-06</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{0}$</t>
+          <t>(h$_{rs}$)$_{1}$</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>2.161522061566603e-06</v>
+        <v>2.090544731761845e-06</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>(h$_{rs}$)$_{1}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>2.034060694932896e-06</v>
+        <v>2.088416151256583e-06</v>
       </c>
     </row>
     <row r="69">
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1.867379770044898e-06</v>
+        <v>1.928148437475984e-06</v>
       </c>
     </row>
     <row r="70">
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1.616492031364258e-06</v>
+        <v>1.614953245947436e-06</v>
       </c>
     </row>
     <row r="71">
@@ -1352,33 +1352,33 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1.541625136547503e-06</v>
+        <v>1.534974687521078e-06</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{1}$</t>
+          <t>$(\eta_{r})_{1}$</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>1.420549705372149e-06</v>
+        <v>1.447370215696673e-06</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{1}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>1.419893049000004e-06</v>
+        <v>1.384610267673221e-06</v>
       </c>
     </row>
     <row r="74">
@@ -1391,7 +1391,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1.331841715321663e-06</v>
+        <v>1.368442915242756e-06</v>
       </c>
     </row>
     <row r="75">
@@ -1404,7 +1404,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1.287323041683143e-06</v>
+        <v>1.288572415691375e-06</v>
       </c>
     </row>
     <row r="76">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>1.1524700653601e-06</v>
+        <v>1.139929265136116e-06</v>
       </c>
     </row>
     <row r="77">
@@ -1430,7 +1430,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>9.693119354045891e-07</v>
+        <v>8.960245586189157e-07</v>
       </c>
     </row>
     <row r="78">
@@ -1443,33 +1443,33 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>7.53046982235866e-07</v>
+        <v>7.311489799564644e-07</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>(h$_{pq}$)$_{0}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>6.791581286895688e-07</v>
+        <v>6.791928301510475e-07</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{3}$</t>
+          <t>(h$_{pq}$)$_{0}$</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>6.365518206814005e-07</v>
+        <v>6.739016698251171e-07</v>
       </c>
     </row>
     <row r="81">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>5.311686981222513e-07</v>
+        <v>5.453312792359722e-07</v>
       </c>
     </row>
     <row r="82">
@@ -1495,7 +1495,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>3.503942292561819e-07</v>
+        <v>3.49406901722563e-07</v>
       </c>
     </row>
     <row r="83">
@@ -1508,7 +1508,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>3.897830628535145e-08</v>
+        <v>2.834373844795528e-08</v>
       </c>
     </row>
     <row r="84">
@@ -1521,7 +1521,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>1.084715341690152e-08</v>
+        <v>9.540340858167671e-09</v>
       </c>
     </row>
     <row r="85">
@@ -1534,72 +1534,72 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>3.229006925045185e-09</v>
+        <v>3.521099726045723e-09</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{2}$</t>
+          <t>$(\omega_{r})_{1}$</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>2.586757821491536e-09</v>
+        <v>2.373144711014198e-09</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
+          <t>$(\omega_{r})_{2}$</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>1.864466745935933e-09</v>
+        <v>2.306757980124273e-09</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{0}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>1.782015059132638e-09</v>
+        <v>2.027877903381537e-09</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{1}$</t>
+          <t>$\omega_{s}$</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1.75481771446811e-09</v>
+        <v>1.981271324415822e-09</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
+          <t>$(\omega_{r})_{0}$</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>1.671646071409022e-09</v>
+        <v>1.427049858443511e-09</v>
       </c>
     </row>
     <row r="91">
@@ -1612,46 +1612,46 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>1.63652090483557e-09</v>
+        <v>1.360869585401551e-09</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>$\omega_{s}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>1.450305140952312e-09</v>
+        <v>1.272613058268239e-09</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>$\omega_{q}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1.06117104656905e-09</v>
+        <v>1.246339974398595e-09</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>87</v>
+        <v>33</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
+          <t>$\omega_{q}$</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1.049725565464064e-09</v>
+        <v>1.229068629982067e-09</v>
       </c>
     </row>
     <row r="95">
@@ -1664,7 +1664,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>2.091820723572891e-10</v>
+        <v>1.7927719694614e-10</v>
       </c>
     </row>
     <row r="96">

</xml_diff>